<commit_message>
update for Sales POC
update for Sales POC
</commit_message>
<xml_diff>
--- a/TestData/dataDriven_sample.xlsx
+++ b/TestData/dataDriven_sample.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CDKproject\autotest\test_selenium_Python3\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macgouyuling/Documents/Usual/CKD/BMWpocTest/TestData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4844277A-65FC-4CCC-9704-130A39215B07}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11B7AFFD-A4B1-A445-9C90-98C04EC5DCDC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9780" yWindow="5780" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestScenario" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="32">
   <si>
     <t>Testcase</t>
   </si>
@@ -46,6 +46,9 @@
     <t>click</t>
   </si>
   <si>
+    <t>takesleep</t>
+  </si>
+  <si>
     <t>screenshot</t>
   </si>
   <si>
@@ -77,6 +80,48 @@
   </si>
   <si>
     <t>Intranet username and password:</t>
+  </si>
+  <si>
+    <t>xpath=//div[@class="card perfect"]/div[1]/div[2]/div/section</t>
+  </si>
+  <si>
+    <t>xpath=//div[@class="card perfect"]/div[1]/div[1]/input</t>
+  </si>
+  <si>
+    <t>xpath=//div[@class="card"]/div[1]/div[1]/input</t>
+  </si>
+  <si>
+    <t>xpath=//div[@class="card"]/div[1]/div[2]/div/section</t>
+  </si>
+  <si>
+    <t>01_perfect_extend.png</t>
+  </si>
+  <si>
+    <t>02_perfect_select.png</t>
+  </si>
+  <si>
+    <t>03_select_confirm.png</t>
+  </si>
+  <si>
+    <t>04_confirm_extend.png</t>
+  </si>
+  <si>
+    <t>05_confirm_select.png</t>
+  </si>
+  <si>
+    <t>06_select_pay.png</t>
+  </si>
+  <si>
+    <t>07_pay_extend.png</t>
+  </si>
+  <si>
+    <t>xpath=//span[text()='订单确认']</t>
+  </si>
+  <si>
+    <t>xpath=//span[text()='确定付款']</t>
+  </si>
+  <si>
+    <t>xpath=//div[@class="card"]/div[1]/div/div/section</t>
   </si>
 </sst>
 </file>
@@ -127,9 +172,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -445,23 +489,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E1048573"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.54296875" customWidth="1"/>
-    <col min="2" max="2" width="16.1796875" customWidth="1"/>
-    <col min="3" max="3" width="73.453125" customWidth="1"/>
-    <col min="4" max="4" width="45.81640625" customWidth="1"/>
-    <col min="5" max="5" width="35.7265625" customWidth="1"/>
-    <col min="6" max="1025" width="8.54296875" customWidth="1"/>
+    <col min="1" max="1" width="21.5" customWidth="1"/>
+    <col min="2" max="2" width="16.1640625" customWidth="1"/>
+    <col min="3" max="3" width="69.6640625" customWidth="1"/>
+    <col min="4" max="4" width="45.83203125" customWidth="1"/>
+    <col min="5" max="5" width="35.6640625" customWidth="1"/>
+    <col min="6" max="1025" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -474,11 +518,223 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="1048573" ht="12.75" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1">
+        <v>1</v>
+      </c>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1">
+        <v>1</v>
+      </c>
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B14" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1">
+        <v>1</v>
+      </c>
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B17" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1">
+        <v>1</v>
+      </c>
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B20" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1">
+        <v>1</v>
+      </c>
+      <c r="E21" s="1"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E22" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -493,99 +749,99 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1025" width="8.54296875" customWidth="1"/>
+    <col min="1" max="1025" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
-      <c r="B1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>7</v>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="2"/>
+        <v>10</v>
+      </c>
+      <c r="D4" s="1"/>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="1"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="1"/>
-      <c r="B6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="1"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="1"/>
-      <c r="B7" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="2"/>
+      <c r="D7" s="1"/>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="2"/>
+        <v>13</v>
+      </c>
+      <c r="D8" s="1"/>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
-      <c r="B9" s="2" t="s">
-        <v>6</v>
+      <c r="B9" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="C9" s="1"/>
-      <c r="D9" s="2" t="s">
-        <v>13</v>
+      <c r="D9" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="E9" s="1"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>